<commit_message>
assembled fisher raw and started plotting histos
</commit_message>
<xml_diff>
--- a/sbs_meta/scraped/Fisher2009/Fisher_2009.xlsx
+++ b/sbs_meta/scraped/Fisher2009/Fisher_2009.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="41380" yWindow="-1220" windowWidth="26860" windowHeight="17680" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11120" windowHeight="12800" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fisher_2009_fig1_edit.csv" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="111">
   <si>
     <t>x</t>
   </si>
@@ -793,6 +793,9 @@
   </si>
   <si>
     <t>n_sites</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -2920,10 +2923,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3073,6 +3076,38 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:6">
+      <c r="E8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <f>SUM(E2:E3)</f>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <f>SUM(E4:E5)</f>
+        <v>692</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <f>SUM(E6:E7)</f>
+        <v>729</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>